<commit_message>
correcoes para a christiane
</commit_message>
<xml_diff>
--- a/docs/AC04 - CHRISTIANE/Analise_de_Eventos_ATENDER_CLIENTE.xlsx
+++ b/docs/AC04 - CHRISTIANE/Analise_de_Eventos_ATENDER_CLIENTE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t xml:space="preserve">Externo</t>
   </si>
@@ -75,7 +75,7 @@
     <t xml:space="preserve">X(1)</t>
   </si>
   <si>
-    <t xml:space="preserve">O garçom solicita o preparo do pedido</t>
+    <t xml:space="preserve">O atendente solicita o preparo do pedido</t>
   </si>
   <si>
     <t xml:space="preserve">X(2)</t>
@@ -84,10 +84,7 @@
     <t xml:space="preserve">A cozinha informa que o pedido está pronto</t>
   </si>
   <si>
-    <t xml:space="preserve">X(3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O copeiro prepara a bebida</t>
+    <t xml:space="preserve">O copeiro entrega a bebida pronta</t>
   </si>
 </sst>
 </file>
@@ -353,7 +350,7 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -486,7 +483,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="15"/>
@@ -496,22 +493,29 @@
     </row>
     <row r="7" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="C7" s="9" t="n">
         <v>5</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
     </row>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>